<commit_message>
print diff 73 days/ 30 = 2
</commit_message>
<xml_diff>
--- a/testdf_final.xlsx
+++ b/testdf_final.xlsx
@@ -530,16 +530,16 @@
         <v>703.9409695767351</v>
       </c>
       <c r="D2" t="n">
-        <v>927.1671217952892</v>
+        <v>932.2017155010354</v>
       </c>
       <c r="E2" t="n">
-        <v>1150.754070505559</v>
+        <v>1143.41330678195</v>
       </c>
       <c r="F2" t="n">
-        <v>703.9409695105414</v>
+        <v>703.940969505364</v>
       </c>
       <c r="G2" t="n">
-        <v>703.9409696455268</v>
+        <v>703.9409696685137</v>
       </c>
       <c r="H2" t="n">
         <v>336.3824876801255</v>

</xml_diff>